<commit_message>
fix: mutiple subjects logic
</commit_message>
<xml_diff>
--- a/data/planilha_teste.xlsx
+++ b/data/planilha_teste.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
   <si>
     <t>Códigos Origem</t>
   </si>
@@ -144,19 +144,7 @@
     <t>Introdução à Programação</t>
   </si>
   <si>
-    <t>Conteúdo programático compatível em mais de 75%.</t>
-  </si>
-  <si>
-    <t>INF1005</t>
-  </si>
-  <si>
-    <t>Lógica Matemática</t>
-  </si>
-  <si>
-    <t>Foco apenas em lógica, falta o conteúdo de Teoria dos Conjuntos.</t>
-  </si>
-  <si>
-    <t>20/05/2024</t>
+    <t>Conteúdo programático compatível.</t>
   </si>
   <si>
     <t>MAT1161</t>
@@ -165,7 +153,7 @@
     <t>Cálculo a Uma Variável</t>
   </si>
   <si>
-    <t>Equivalência já conhecida pela comissão.</t>
+    <t>Equivalência já conhecida.</t>
   </si>
   <si>
     <t>15/02/2023</t>
@@ -183,10 +171,46 @@
     <t>Programação Orientada a Objetos</t>
   </si>
   <si>
-    <t>A combinação das duas ementas cobre os paradigmas e ferramentas ensinados em POO.</t>
+    <t>TESTE (Muitos-para-Um) A combinação cobre os paradigmas de POO.</t>
   </si>
   <si>
     <t>Adriana</t>
+  </si>
+  <si>
+    <t>INF1300</t>
+  </si>
+  <si>
+    <t>Algoritmos Avançados</t>
+  </si>
+  <si>
+    <t>ICP241+ICP242</t>
+  </si>
+  <si>
+    <t>Estrutura de Dados + Grafos</t>
+  </si>
+  <si>
+    <t>TESTE (Um-para-Muitos) Cobre ambas as ementas.</t>
+  </si>
+  <si>
+    <t>Juliana França</t>
+  </si>
+  <si>
+    <t>INF1301+INF1302</t>
+  </si>
+  <si>
+    <t>Lógica Aplicada + Teoria da Computação</t>
+  </si>
+  <si>
+    <t>ICP370+ICP123</t>
+  </si>
+  <si>
+    <t>Lógica para Computação + Linguagens Formais</t>
+  </si>
+  <si>
+    <t>TESTE (Muitos-para-Muitos) Combinação favorável.</t>
+  </si>
+  <si>
+    <t>15/05/2025</t>
   </si>
   <si>
     <t>GMA00167</t>
@@ -3842,22 +3866,22 @@
         <v>45</v>
       </c>
       <c r="C3" s="10">
-        <v>60.0</v>
+        <v>90.0</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>46</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>47</v>
@@ -3871,83 +3895,83 @@
         <v>49</v>
       </c>
       <c r="C4" s="10">
-        <v>90.0</v>
+        <v>120.0</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="I4" s="13">
+        <v>45607.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C5" s="10">
-        <v>120.0</v>
+        <v>60.0</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="13">
-        <v>45607.0</v>
+        <v>59</v>
+      </c>
+      <c r="I5" s="11">
+        <v>45931.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="4">
-        <v>60.0</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="A6" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="10">
+        <v>120.0</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>35</v>
+      <c r="I6" s="9" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7">
@@ -7000,7 +7024,7 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>26</v>
@@ -7018,10 +7042,10 @@
         <v>26</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="I2" s="11">
         <v>45783.0</v>
@@ -7029,10 +7053,10 @@
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C3" s="10">
         <v>75.0</v>
@@ -7047,7 +7071,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>15</v>
@@ -7058,10 +7082,10 @@
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C4" s="10">
         <v>60.0</v>
@@ -7070,27 +7094,27 @@
         <v>30</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>34</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C5" s="10">
         <v>90.0</v>
@@ -7099,19 +7123,19 @@
         <v>11</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6">

</xml_diff>